<commit_message>
remove entries where neither rate nor bool is given
</commit_message>
<xml_diff>
--- a/data/lit/20201218_UGT_activitydata_from_lit.xlsx
+++ b/data/lit/20201218_UGT_activitydata_from_lit.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cdmadsen/GT/data/lit/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47F7540B-1D59-0240-AF6D-2E7BA899A2E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3700B01C-D377-8B4A-A6B3-1776DFD7F1E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1460" yWindow="700" windowWidth="27520" windowHeight="19600" xr2:uid="{8E669582-CF78-574E-ADA5-8030D83D9794}"/>
+    <workbookView xWindow="4740" yWindow="5140" windowWidth="27520" windowHeight="19600" xr2:uid="{8E669582-CF78-574E-ADA5-8030D83D9794}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -199,9 +199,6 @@
     <t>Reactive</t>
   </si>
   <si>
-    <t>ProteinName</t>
-  </si>
-  <si>
     <t>KcatPerSecStd</t>
   </si>
   <si>
@@ -374,6 +371,9 @@
   </si>
   <si>
     <t>0.0183333333333333</t>
+  </si>
+  <si>
+    <t>Protein</t>
   </si>
 </sst>
 </file>
@@ -1170,7 +1170,7 @@
   <dimension ref="A1:G94"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1189,10 +1189,10 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>54</v>
+        <v>112</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>20</v>
@@ -1201,13 +1201,13 @@
         <v>53</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -1221,16 +1221,16 @@
         <v>0</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>67</v>
-      </c>
       <c r="G2" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -1244,16 +1244,16 @@
         <v>1</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -1264,19 +1264,19 @@
         <v>21</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>70</v>
-      </c>
       <c r="G4" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -1290,16 +1290,16 @@
         <v>18</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -1313,16 +1313,16 @@
         <v>2</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -1336,16 +1336,16 @@
         <v>3</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -1359,16 +1359,16 @@
         <v>4</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -1382,16 +1382,16 @@
         <v>5</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -1405,16 +1405,16 @@
         <v>6</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -1428,16 +1428,16 @@
         <v>7</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -1451,16 +1451,16 @@
         <v>8</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -1474,16 +1474,16 @@
         <v>9</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E13" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="F13" s="1" t="s">
-        <v>72</v>
-      </c>
       <c r="G13" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -1497,16 +1497,16 @@
         <v>10</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -1520,16 +1520,16 @@
         <v>11</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E15" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F15" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="F15" s="1" t="s">
-        <v>74</v>
-      </c>
       <c r="G15" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -1543,16 +1543,16 @@
         <v>12</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -1566,16 +1566,16 @@
         <v>13</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -1589,16 +1589,16 @@
         <v>14</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -1609,19 +1609,19 @@
         <v>21</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -1635,16 +1635,16 @@
         <v>19</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
@@ -1658,16 +1658,16 @@
         <v>15</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
@@ -1681,16 +1681,16 @@
         <v>16</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
@@ -1701,19 +1701,19 @@
         <v>21</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
@@ -1727,16 +1727,16 @@
         <v>28</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
@@ -1750,16 +1750,16 @@
         <v>28</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
@@ -1773,16 +1773,16 @@
         <v>28</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
@@ -1796,16 +1796,16 @@
         <v>28</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
@@ -1813,22 +1813,22 @@
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>28</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
@@ -1836,22 +1836,22 @@
         <v>22</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>28</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
@@ -1862,19 +1862,19 @@
         <v>35</v>
       </c>
       <c r="C30" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E30" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="D30" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>83</v>
-      </c>
       <c r="F30" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
@@ -1885,19 +1885,19 @@
         <v>36</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
@@ -1908,19 +1908,19 @@
         <v>37</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
@@ -1931,19 +1931,19 @@
         <v>38</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
@@ -1951,22 +1951,22 @@
         <v>27</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
@@ -1974,22 +1974,22 @@
         <v>22</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
@@ -2000,19 +2000,19 @@
         <v>35</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
@@ -2023,19 +2023,19 @@
         <v>36</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
@@ -2046,19 +2046,19 @@
         <v>37</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
@@ -2069,19 +2069,19 @@
         <v>38</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
@@ -2089,22 +2089,22 @@
         <v>27</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
@@ -2112,22 +2112,22 @@
         <v>22</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
@@ -2141,16 +2141,16 @@
         <v>29</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
@@ -2164,16 +2164,16 @@
         <v>29</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
@@ -2187,16 +2187,16 @@
         <v>29</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
@@ -2210,16 +2210,16 @@
         <v>29</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
@@ -2227,22 +2227,22 @@
         <v>27</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>29</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
@@ -2250,22 +2250,22 @@
         <v>22</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>29</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
@@ -2279,16 +2279,16 @@
         <v>30</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
@@ -2302,16 +2302,16 @@
         <v>30</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
@@ -2325,16 +2325,16 @@
         <v>30</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
@@ -2348,16 +2348,16 @@
         <v>30</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
@@ -2365,22 +2365,22 @@
         <v>27</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>30</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
@@ -2388,22 +2388,22 @@
         <v>22</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>30</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
@@ -2417,16 +2417,16 @@
         <v>31</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
@@ -2440,16 +2440,16 @@
         <v>31</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
@@ -2463,16 +2463,16 @@
         <v>31</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
@@ -2486,16 +2486,16 @@
         <v>31</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
@@ -2503,22 +2503,22 @@
         <v>27</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>31</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
@@ -2526,22 +2526,22 @@
         <v>22</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>31</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
@@ -2555,16 +2555,16 @@
         <v>32</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
@@ -2578,16 +2578,16 @@
         <v>32</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G61" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
@@ -2601,16 +2601,16 @@
         <v>32</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
@@ -2624,16 +2624,16 @@
         <v>32</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G63" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
@@ -2641,22 +2641,22 @@
         <v>27</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>32</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G64" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
@@ -2664,22 +2664,22 @@
         <v>22</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>32</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G65" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
@@ -2693,16 +2693,16 @@
         <v>33</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G66" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
@@ -2716,16 +2716,16 @@
         <v>33</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G67" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
@@ -2739,16 +2739,16 @@
         <v>33</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G68" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
@@ -2762,16 +2762,16 @@
         <v>33</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G69" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
@@ -2779,22 +2779,22 @@
         <v>27</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G70" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
@@ -2802,22 +2802,22 @@
         <v>22</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G71" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.2">
@@ -2831,16 +2831,16 @@
         <v>34</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G72" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
@@ -2854,16 +2854,16 @@
         <v>34</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G73" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
@@ -2877,16 +2877,16 @@
         <v>34</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G74" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
@@ -2900,16 +2900,16 @@
         <v>34</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G75" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.2">
@@ -2917,22 +2917,22 @@
         <v>27</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>34</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G76" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.2">
@@ -2940,22 +2940,22 @@
         <v>22</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>34</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G77" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.2">
@@ -2963,22 +2963,22 @@
         <v>39</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>40</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E78" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F78" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="F78" s="1" t="s">
-        <v>90</v>
-      </c>
       <c r="G78" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.2">
@@ -2986,114 +2986,114 @@
         <v>39</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>41</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E79" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F79" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="F79" s="1" t="s">
-        <v>92</v>
-      </c>
       <c r="G79" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>40</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>41</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>40</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E82" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F82" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="F82" s="1" t="s">
-        <v>95</v>
-      </c>
       <c r="G82" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>41</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G83" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.2">
@@ -3101,22 +3101,22 @@
         <v>39</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>42</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E84" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="F84" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="F84" s="1" t="s">
-        <v>98</v>
-      </c>
       <c r="G84" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.2">
@@ -3124,22 +3124,22 @@
         <v>39</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>43</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G85" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.2">
@@ -3147,22 +3147,22 @@
         <v>39</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>44</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G86" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.2">
@@ -3170,22 +3170,22 @@
         <v>39</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>45</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E87" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="F87" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="F87" s="1" t="s">
-        <v>102</v>
-      </c>
       <c r="G87" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
@@ -3193,22 +3193,22 @@
         <v>39</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>46</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G88" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.2">
@@ -3216,22 +3216,22 @@
         <v>39</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>47</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E89" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F89" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="F89" s="1" t="s">
-        <v>105</v>
-      </c>
       <c r="G89" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.2">
@@ -3239,22 +3239,22 @@
         <v>39</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C90" s="1" t="s">
         <v>48</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G90" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.2">
@@ -3262,22 +3262,22 @@
         <v>39</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C91" s="1" t="s">
         <v>49</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G91" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.2">
@@ -3285,22 +3285,22 @@
         <v>39</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C92" s="1" t="s">
         <v>50</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G92" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.2">
@@ -3308,22 +3308,22 @@
         <v>39</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C93" s="1" t="s">
         <v>51</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E93" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F93" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="F93" s="1" t="s">
-        <v>110</v>
-      </c>
       <c r="G93" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.2">
@@ -3331,22 +3331,22 @@
         <v>39</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C94" s="1" t="s">
         <v>52</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E94" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F94" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="F94" s="1" t="s">
-        <v>112</v>
-      </c>
       <c r="G94" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -3362,12 +3362,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3517,15 +3514,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{25D8D9F4-D941-4B30-B926-C9466D8FCA83}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{55014E57-9161-4625-AEE8-D33CCFECDBA5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3549,10 +3550,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{55014E57-9161-4625-AEE8-D33CCFECDBA5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{25D8D9F4-D941-4B30-B926-C9466D8FCA83}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>